<commit_message>
Update assembly information and add sourcelink support
- Updated AssemblyInformationalVersion to include commit hash.
- Modified AssemblyInfoInputs.cache and CoreCompileInputs.cache for updated inputs.
- Added ConsoleApp1.sourcelink.json for source linking.
- Updated binary files: ConsoleApp1.dll, ConsoleApp1.pdb, apphost.exe, and reference assemblies.
</commit_message>
<xml_diff>
--- a/Alarms.xlsx
+++ b/Alarms.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="10" documentId="11_0E5B5F756691EFF7F89183356559787FC173C573" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F1F2F42-A346-4528-8FD3-BABBB66DCFDC}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MiscInput" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,21 @@
     <sheet name="Motor" sheetId="3" r:id="rId3"/>
     <sheet name="Reference_Sheet" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1278,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
-      <selection sqref="A1:M1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>